<commit_message>
Agregando la funcion que corrije detalles de comparacion - unificando las funciones en un solo bloque de codigo
</commit_message>
<xml_diff>
--- a/Comparacion1.xlsx
+++ b/Comparacion1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>producto</t>
   </si>
@@ -40,42 +40,30 @@
     <t>Metro</t>
   </si>
   <si>
+    <t>AZUCAR RUBIA//AZUCAR RUBIA//AZUCAR RUBIA</t>
+  </si>
+  <si>
     <t>AZUCAR RUBIA//AZUCAR RUBIA</t>
   </si>
   <si>
-    <t>AZUCAR RUBIA//AZUCAR RUBIA//AZUCAR RUBIA</t>
-  </si>
-  <si>
     <t>DULFINA</t>
   </si>
   <si>
-    <t>COSTEÑO</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>KG</t>
   </si>
   <si>
     <t>BOLSA</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>21.90</t>
   </si>
   <si>
-    <t>5.90</t>
-  </si>
-  <si>
     <t>4.89</t>
   </si>
   <si>
@@ -85,16 +73,10 @@
     <t>5.2</t>
   </si>
   <si>
-    <t>9.5</t>
-  </si>
-  <si>
     <t>26.45</t>
   </si>
   <si>
     <t>5.70</t>
-  </si>
-  <si>
-    <t>10.90</t>
   </si>
 </sst>
 </file>
@@ -452,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,22 +474,22 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -518,53 +500,53 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -573,175 +555,19 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
       <c r="H5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" t="s">
         <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>